<commit_message>
Fixes some datasets Improves regionalization of activities
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-biogas.xlsx
+++ b/premise/data/additional_inventories/lci-biogas.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A8039BC-66FC-9D4D-BD72-67D75B444E1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C7FCA3F-B431-CE40-B25A-AE3DFE004D85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34320" yWindow="3080" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Biogas" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1" iterateCount="10" calcOnSave="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="115">
   <si>
     <t>Activity</t>
   </si>
@@ -229,12 +229,6 @@
     <t>biogas</t>
   </si>
   <si>
-    <t>code</t>
-  </si>
-  <si>
-    <t>5baf9cc755ef7bd3bea235d9fb6e0cb8</t>
-  </si>
-  <si>
     <t>worksheet name</t>
   </si>
   <si>
@@ -307,9 +301,6 @@
     <t>market for NOx retained, by selective catalytic reduction</t>
   </si>
   <si>
-    <t>Nox retained, by selective catalytic reduction</t>
-  </si>
-  <si>
     <t>market for steam, in chemical industry</t>
   </si>
   <si>
@@ -383,6 +374,9 @@
   </si>
   <si>
     <t>natural resource::in air</t>
+  </si>
+  <si>
+    <t>NOx retained, by selective catalytic reduction</t>
   </si>
 </sst>
 </file>
@@ -774,10 +768,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M102"/>
+  <dimension ref="A1:M101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="F69" sqref="F69"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="A87" sqref="A87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -804,7 +798,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -828,7 +822,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -836,7 +830,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -849,10 +843,10 @@
     </row>
     <row r="9" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -888,7 +882,7 @@
     </row>
     <row r="12" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B12" s="6">
         <v>1</v>
@@ -907,12 +901,12 @@
         <v>31</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B13" s="6">
         <v>6.4290000000000003</v>
@@ -924,13 +918,13 @@
         <v>59</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>36</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -938,7 +932,7 @@
         <v>0</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -962,7 +956,7 @@
         <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
@@ -970,7 +964,7 @@
         <v>14</v>
       </c>
       <c r="B21" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -978,15 +972,15 @@
         <v>7</v>
       </c>
       <c r="B22" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B23" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -1022,7 +1016,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -1034,18 +1028,18 @@
         <v>59</v>
       </c>
       <c r="E26" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G26" t="s">
         <v>31</v>
       </c>
       <c r="H26" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B27" s="2">
         <v>2.0100000000000001E-12</v>
@@ -1063,12 +1057,12 @@
         <v>36</v>
       </c>
       <c r="H27" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B28">
         <v>5.2900000000000003E-2</v>
@@ -1086,12 +1080,12 @@
         <v>36</v>
       </c>
       <c r="H28" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B29" s="2">
         <v>7.7000000000000001E-5</v>
@@ -1109,12 +1103,12 @@
         <v>36</v>
       </c>
       <c r="H29" t="s">
-        <v>91</v>
+        <v>114</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B30" s="2">
         <v>6.3899999999999995E-5</v>
@@ -1132,7 +1126,7 @@
         <v>36</v>
       </c>
       <c r="H30" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -1146,7 +1140,7 @@
         <v>34</v>
       </c>
       <c r="D31" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E31" t="s">
         <v>53</v>
@@ -1184,7 +1178,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B33" s="2">
         <v>5.8799999999999998E-3</v>
@@ -1204,7 +1198,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B34" s="2">
         <v>5.2699999999999999E-7</v>
@@ -1224,7 +1218,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B35" s="2">
         <v>1.36E-5</v>
@@ -1244,7 +1238,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B36" s="2">
         <v>1.4499999999999999E-7</v>
@@ -1270,7 +1264,7 @@
         <v>0</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
@@ -1294,7 +1288,7 @@
         <v>6</v>
       </c>
       <c r="B41" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
@@ -1302,7 +1296,7 @@
         <v>14</v>
       </c>
       <c r="B42" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
@@ -1315,10 +1309,10 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B44" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
@@ -1326,7 +1320,7 @@
         <v>2</v>
       </c>
       <c r="B45" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -1362,7 +1356,7 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B48">
         <v>1</v>
@@ -1380,7 +1374,7 @@
         <v>31</v>
       </c>
       <c r="H48" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
@@ -1432,7 +1426,7 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B51">
         <f>0.061874*0.669</f>
@@ -1445,18 +1439,18 @@
         <v>4</v>
       </c>
       <c r="F51" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G51" t="s">
         <v>36</v>
       </c>
       <c r="H51" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B52">
         <f>0.000000034944*0.669</f>
@@ -1466,21 +1460,21 @@
         <v>34</v>
       </c>
       <c r="D52" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F52" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G52" t="s">
         <v>36</v>
       </c>
       <c r="H52" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B53" s="2">
         <v>8.4800000000000005E-8</v>
@@ -1498,12 +1492,12 @@
         <v>36</v>
       </c>
       <c r="H53" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B54">
         <f>(0.00000521*0.669)+0.000010376</f>
@@ -1566,7 +1560,7 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B57">
         <f>0.0000018*0.669</f>
@@ -1598,7 +1592,7 @@
         <v>2</v>
       </c>
       <c r="B60" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
@@ -1635,10 +1629,10 @@
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B65" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="66" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -1706,7 +1700,7 @@
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B69">
         <v>1.3713596052052344</v>
@@ -1729,7 +1723,7 @@
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B70" s="2">
         <f>2.65+B69</f>
@@ -1742,16 +1736,16 @@
         <v>8</v>
       </c>
       <c r="F70" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G70" t="s">
         <v>20</v>
       </c>
       <c r="H70" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="I70" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
@@ -2002,7 +1996,7 @@
         <v>34</v>
       </c>
       <c r="D80" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E80" t="s">
         <v>8</v>
@@ -2100,7 +2094,7 @@
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B84">
         <v>55.5</v>
@@ -2109,10 +2103,10 @@
         <v>18</v>
       </c>
       <c r="E84" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F84" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G84" t="s">
         <v>20</v>
@@ -2128,144 +2122,162 @@
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>65</v>
+        <v>3</v>
       </c>
       <c r="B87" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>3</v>
-      </c>
-      <c r="B88" t="s">
-        <v>59</v>
+        <v>5</v>
+      </c>
+      <c r="B88">
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>5</v>
-      </c>
-      <c r="B89">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="B89" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B90" t="s">
-        <v>58</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="M90" s="2"/>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="B91" t="s">
-        <v>8</v>
-      </c>
-      <c r="M91" s="2"/>
+        <v>30</v>
+      </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="B92" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
-        <v>80</v>
-      </c>
-      <c r="B93" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="94" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A94" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A93" s="1" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>10</v>
+      </c>
+      <c r="B94" t="s">
+        <v>11</v>
+      </c>
+      <c r="C94" t="s">
+        <v>12</v>
+      </c>
+      <c r="D94" t="s">
+        <v>3</v>
+      </c>
+      <c r="E94" t="s">
+        <v>7</v>
+      </c>
+      <c r="F94" t="s">
+        <v>14</v>
+      </c>
+      <c r="G94" t="s">
+        <v>66</v>
+      </c>
+      <c r="H94" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>10</v>
-      </c>
-      <c r="B95" t="s">
-        <v>11</v>
+        <v>58</v>
+      </c>
+      <c r="B95">
+        <v>1</v>
       </c>
       <c r="C95" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="D95" t="s">
-        <v>3</v>
+        <v>59</v>
       </c>
       <c r="E95" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F95" t="s">
-        <v>14</v>
-      </c>
-      <c r="G95" t="s">
-        <v>68</v>
+        <v>31</v>
       </c>
       <c r="H95" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="B96">
-        <v>1</v>
+        <v>2.3800000000000001E-4</v>
       </c>
       <c r="C96" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D96" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="E96" t="s">
-        <v>8</v>
+        <v>69</v>
       </c>
       <c r="F96" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="H96" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B97">
-        <v>2.3800000000000001E-4</v>
+        <v>3.4339655648031599E-10</v>
       </c>
       <c r="C97" t="s">
         <v>34</v>
       </c>
       <c r="D97" t="s">
-        <v>70</v>
+        <v>35</v>
       </c>
       <c r="E97" t="s">
-        <v>71</v>
+        <v>8</v>
       </c>
       <c r="F97" t="s">
         <v>36</v>
       </c>
+      <c r="G97" t="s">
+        <v>72</v>
+      </c>
       <c r="H97" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B98">
-        <v>3.4339655648031599E-10</v>
+        <v>1.8660000000000003E-2</v>
       </c>
       <c r="C98" t="s">
         <v>34</v>
@@ -2278,9 +2290,6 @@
       </c>
       <c r="F98" t="s">
         <v>36</v>
-      </c>
-      <c r="G98" t="s">
-        <v>74</v>
       </c>
       <c r="H98" t="s">
         <v>75</v>
@@ -2291,7 +2300,7 @@
         <v>76</v>
       </c>
       <c r="B99">
-        <v>1.8660000000000003E-2</v>
+        <v>8.1000000000000013E-3</v>
       </c>
       <c r="C99" t="s">
         <v>34</v>
@@ -2311,16 +2320,16 @@
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>78</v>
+        <v>50</v>
       </c>
       <c r="B100">
-        <v>8.1000000000000013E-3</v>
+        <v>0.996</v>
       </c>
       <c r="C100" t="s">
         <v>34</v>
       </c>
       <c r="D100" t="s">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="E100" t="s">
         <v>8</v>
@@ -2329,52 +2338,29 @@
         <v>36</v>
       </c>
       <c r="H100" t="s">
-        <v>79</v>
+        <v>51</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B101">
-        <v>0.996</v>
+        <v>3.44E-2</v>
       </c>
       <c r="C101" t="s">
         <v>34</v>
       </c>
       <c r="D101" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="E101" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="F101" t="s">
         <v>36</v>
       </c>
       <c r="H101" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A102" t="s">
-        <v>52</v>
-      </c>
-      <c r="B102">
-        <v>3.44E-2</v>
-      </c>
-      <c r="C102" t="s">
-        <v>34</v>
-      </c>
-      <c r="D102" t="s">
-        <v>59</v>
-      </c>
-      <c r="E102" t="s">
-        <v>53</v>
-      </c>
-      <c r="F102" t="s">
-        <v>36</v>
-      </c>
-      <c r="H102" t="s">
         <v>56</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update relative to master branch
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-biogas.xlsx
+++ b/premise/data/additional_inventories/lci-biogas.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC1B9947-C183-EE45-B371-753590952357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A8039BC-66FC-9D4D-BD72-67D75B444E1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Biogas" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1" iterateCount="10" calcOnSave="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -220,6 +220,9 @@
     <t>2 wt-% potassium iodide solution</t>
   </si>
   <si>
+    <t>treatment of sewage sludge by anaerobic digestion</t>
+  </si>
+  <si>
     <t>cubic meter</t>
   </si>
   <si>
@@ -304,6 +307,9 @@
     <t>market for NOx retained, by selective catalytic reduction</t>
   </si>
   <si>
+    <t>Nox retained, by selective catalytic reduction</t>
+  </si>
+  <si>
     <t>market for steam, in chemical industry</t>
   </si>
   <si>
@@ -367,22 +373,16 @@
     <t>natural resource::biotic</t>
   </si>
   <si>
+    <t>heat and power co-generation, biogas, gas engine</t>
+  </si>
+  <si>
+    <t>heat, central or small-scale, other than natural gas</t>
+  </si>
+  <si>
     <t>Carbon dioxide, in air</t>
   </si>
   <si>
     <t>natural resource::in air</t>
-  </si>
-  <si>
-    <t>NOx retained, by selective catalytic reduction</t>
-  </si>
-  <si>
-    <t>market for biogas</t>
-  </si>
-  <si>
-    <t>market for heat, central or small-scale, biomethane</t>
-  </si>
-  <si>
-    <t>heat, central or small-scale, biomethane</t>
   </si>
 </sst>
 </file>
@@ -776,8 +776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="F69" sqref="F69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -793,7 +793,7 @@
         <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -804,7 +804,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -828,7 +828,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -836,7 +836,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -849,10 +849,10 @@
     </row>
     <row r="9" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -888,7 +888,7 @@
     </row>
     <row r="12" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B12" s="6">
         <v>1</v>
@@ -907,12 +907,12 @@
         <v>31</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B13" s="6">
         <v>6.4290000000000003</v>
@@ -924,13 +924,13 @@
         <v>59</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>36</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -938,7 +938,7 @@
         <v>0</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -962,7 +962,7 @@
         <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
@@ -970,7 +970,7 @@
         <v>14</v>
       </c>
       <c r="B21" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -978,15 +978,15 @@
         <v>7</v>
       </c>
       <c r="B22" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B23" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -1022,7 +1022,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -1034,18 +1034,18 @@
         <v>59</v>
       </c>
       <c r="E26" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G26" t="s">
         <v>31</v>
       </c>
       <c r="H26" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B27" s="2">
         <v>2.0100000000000001E-12</v>
@@ -1063,12 +1063,12 @@
         <v>36</v>
       </c>
       <c r="H27" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B28">
         <v>5.2900000000000003E-2</v>
@@ -1086,12 +1086,12 @@
         <v>36</v>
       </c>
       <c r="H28" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B29" s="2">
         <v>7.7000000000000001E-5</v>
@@ -1109,12 +1109,12 @@
         <v>36</v>
       </c>
       <c r="H29" t="s">
-        <v>113</v>
+        <v>91</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B30" s="2">
         <v>6.3899999999999995E-5</v>
@@ -1132,7 +1132,7 @@
         <v>36</v>
       </c>
       <c r="H30" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -1146,7 +1146,7 @@
         <v>34</v>
       </c>
       <c r="D31" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E31" t="s">
         <v>53</v>
@@ -1184,7 +1184,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B33" s="2">
         <v>5.8799999999999998E-3</v>
@@ -1204,7 +1204,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B34" s="2">
         <v>5.2699999999999999E-7</v>
@@ -1224,7 +1224,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B35" s="2">
         <v>1.36E-5</v>
@@ -1244,7 +1244,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B36" s="2">
         <v>1.4499999999999999E-7</v>
@@ -1270,7 +1270,7 @@
         <v>0</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
@@ -1294,7 +1294,7 @@
         <v>6</v>
       </c>
       <c r="B41" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
@@ -1302,7 +1302,7 @@
         <v>14</v>
       </c>
       <c r="B42" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
@@ -1315,10 +1315,10 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B44" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
@@ -1326,7 +1326,7 @@
         <v>2</v>
       </c>
       <c r="B45" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -1362,13 +1362,13 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B48">
         <v>1</v>
       </c>
       <c r="C48" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D48" t="s">
         <v>59</v>
@@ -1380,7 +1380,7 @@
         <v>31</v>
       </c>
       <c r="H48" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
@@ -1391,7 +1391,7 @@
         <v>1.02</v>
       </c>
       <c r="C49" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D49" t="s">
         <v>59</v>
@@ -1432,7 +1432,7 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B51">
         <f>0.061874*0.669</f>
@@ -1445,18 +1445,18 @@
         <v>4</v>
       </c>
       <c r="F51" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G51" t="s">
         <v>36</v>
       </c>
       <c r="H51" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B52">
         <f>0.000000034944*0.669</f>
@@ -1466,21 +1466,21 @@
         <v>34</v>
       </c>
       <c r="D52" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F52" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="G52" t="s">
         <v>36</v>
       </c>
       <c r="H52" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B53" s="2">
         <v>8.4800000000000005E-8</v>
@@ -1498,12 +1498,12 @@
         <v>36</v>
       </c>
       <c r="H53" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B54">
         <f>(0.00000521*0.669)+0.000010376</f>
@@ -1566,7 +1566,7 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B57">
         <f>0.0000018*0.669</f>
@@ -1598,7 +1598,7 @@
         <v>2</v>
       </c>
       <c r="B60" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
@@ -1635,10 +1635,10 @@
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B65" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="66" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -1706,7 +1706,7 @@
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B69">
         <v>1.3713596052052344</v>
@@ -1729,7 +1729,7 @@
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="B70" s="2">
         <f>2.65+B69</f>
@@ -1742,16 +1742,16 @@
         <v>8</v>
       </c>
       <c r="F70" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="G70" t="s">
         <v>20</v>
       </c>
       <c r="H70" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I70" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
@@ -2002,7 +2002,7 @@
         <v>34</v>
       </c>
       <c r="D80" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E80" t="s">
         <v>8</v>
@@ -2077,7 +2077,7 @@
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>114</v>
+        <v>62</v>
       </c>
       <c r="B83" s="2">
         <v>2.20868750418312</v>
@@ -2089,18 +2089,18 @@
         <v>4</v>
       </c>
       <c r="E83" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G83" t="s">
         <v>36</v>
       </c>
       <c r="J83" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B84">
         <v>55.5</v>
@@ -2109,10 +2109,10 @@
         <v>18</v>
       </c>
       <c r="E84" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F84" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="G84" t="s">
         <v>20</v>
@@ -2128,10 +2128,10 @@
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B87" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.2">
@@ -2155,7 +2155,7 @@
         <v>6</v>
       </c>
       <c r="B90" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.2">
@@ -2169,7 +2169,7 @@
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B92" t="s">
         <v>30</v>
@@ -2177,10 +2177,10 @@
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B93" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="94" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -2208,7 +2208,7 @@
         <v>14</v>
       </c>
       <c r="G95" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H95" t="s">
         <v>6</v>
@@ -2239,7 +2239,7 @@
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B97">
         <v>2.3800000000000001E-4</v>
@@ -2248,21 +2248,21 @@
         <v>34</v>
       </c>
       <c r="D97" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E97" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F97" t="s">
         <v>36</v>
       </c>
       <c r="H97" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B98">
         <v>3.4339655648031599E-10</v>
@@ -2280,15 +2280,15 @@
         <v>36</v>
       </c>
       <c r="G98" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H98" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B99">
         <v>1.8660000000000003E-2</v>
@@ -2306,12 +2306,12 @@
         <v>36</v>
       </c>
       <c r="H99" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B100">
         <v>8.1000000000000013E-3</v>
@@ -2329,7 +2329,7 @@
         <v>36</v>
       </c>
       <c r="H100" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
@@ -2343,7 +2343,7 @@
         <v>34</v>
       </c>
       <c r="D101" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E101" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Fix issue with fuel mix in IMAGE scenarios Introduce battery and hydrogen storage Add vanadium LCIs
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-biogas.xlsx
+++ b/premise/data/additional_inventories/lci-biogas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5B8301E-E141-3548-99EE-F161FAFCC8A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9CA744B-C2F3-6444-A675-B7DFFA5938BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="162">
   <si>
     <t>Activity</t>
   </si>
@@ -493,12 +493,6 @@
     <t>sodium hydroxide, without water, in 50% solution state</t>
   </si>
   <si>
-    <t>market for water, decarbonised, at user</t>
-  </si>
-  <si>
-    <t>water, decarbonised, at user</t>
-  </si>
-  <si>
     <t>treatment of residue from cooling tower, sanitary landfill</t>
   </si>
   <si>
@@ -515,6 +509,15 @@
   </si>
   <si>
     <t>Biomethane-fired, Combined Cycle. 420 MWel. 7500 full load hours per year. 25 years lifetime. 62% net electrical efficiency.</t>
+  </si>
+  <si>
+    <t>market for water, decarbonised</t>
+  </si>
+  <si>
+    <t>water, decarbonised</t>
+  </si>
+  <si>
+    <t>RoW</t>
   </si>
 </sst>
 </file>
@@ -901,8 +904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -929,7 +932,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M3" t="s">
         <v>108</v>
@@ -962,7 +965,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -970,7 +973,7 @@
         <v>79</v>
       </c>
       <c r="B7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -2044,13 +2047,13 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="B41">
         <v>2.9049999999999998</v>
       </c>
       <c r="C41" t="s">
-        <v>34</v>
+        <v>161</v>
       </c>
       <c r="D41" t="s">
         <v>7</v>
@@ -2077,7 +2080,7 @@
         <v>0</v>
       </c>
       <c r="M41" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
@@ -2121,7 +2124,7 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B43">
         <v>-5.8099999999999994E-6</v>
@@ -2133,7 +2136,7 @@
         <v>7</v>
       </c>
       <c r="E43" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F43" t="s">
         <v>35</v>
@@ -2154,7 +2157,7 @@
         <v>0</v>
       </c>
       <c r="M43" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Fixes external scenario issue
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-biogas.xlsx
+++ b/premise/data/additional_inventories/lci-biogas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B456EAB-33A6-D94E-BEBA-3CE2BCD158D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C7904B8-7C30-B545-AABD-E7C528277CE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34720" yWindow="160" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Biogas" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="159">
   <si>
     <t>Activity</t>
   </si>
@@ -277,12 +277,6 @@
     <t>Life cycle assessment of power-to-gas with biogas as the carbon source, Zhang et al., 2020, Sustainable Energy and Fuels, https://doi.org/10.1039/C9SE00986H</t>
   </si>
   <si>
-    <t>Carbon content of gas uptaken</t>
-  </si>
-  <si>
-    <t>Raw biogas volume * density * 67% CH4 * (16/12) + 32% CO2 * (44/12)</t>
-  </si>
-  <si>
     <t>process</t>
   </si>
   <si>
@@ -338,12 +332,6 @@
   </si>
   <si>
     <t>heat, central or small-scale, other than natural gas</t>
-  </si>
-  <si>
-    <t>Carbon dioxide, in air</t>
-  </si>
-  <si>
-    <t>natural resource::in air</t>
   </si>
   <si>
     <t>biomethane production, from biogas upgrading, using amine scrubbing</t>
@@ -905,10 +893,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N109"/>
+  <dimension ref="A1:N108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="L91" sqref="L91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -935,10 +923,10 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="M3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
@@ -949,7 +937,7 @@
         <v>58</v>
       </c>
       <c r="M4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -960,7 +948,7 @@
         <v>1</v>
       </c>
       <c r="M5" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -968,7 +956,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -976,7 +964,7 @@
         <v>79</v>
       </c>
       <c r="B7" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
@@ -984,10 +972,10 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="M8" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
@@ -995,10 +983,10 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="M9" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
@@ -1009,7 +997,7 @@
         <v>52</v>
       </c>
       <c r="M10" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -1017,7 +1005,7 @@
         <v>8</v>
       </c>
       <c r="M11" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
@@ -1040,25 +1028,25 @@
         <v>13</v>
       </c>
       <c r="G12" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="H12" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="I12" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="J12" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="K12" t="s">
         <v>1</v>
       </c>
       <c r="L12" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="M12" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="N12" t="s">
         <v>5</v>
@@ -1066,7 +1054,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -1078,7 +1066,7 @@
         <v>52</v>
       </c>
       <c r="E13" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="F13" t="s">
         <v>30</v>
@@ -1087,18 +1075,18 @@
         <v>100</v>
       </c>
       <c r="K13" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="L13" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="N13" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B14">
         <v>4.6073299999999991E-12</v>
@@ -1107,7 +1095,7 @@
         <v>7</v>
       </c>
       <c r="E14" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F14" t="s">
         <v>19</v>
@@ -1136,18 +1124,18 @@
         <v>0.80471895621705025</v>
       </c>
       <c r="L14" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="M14">
         <v>0</v>
       </c>
       <c r="N14" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B15">
         <v>4.6479999999999997E-9</v>
@@ -1156,7 +1144,7 @@
         <v>7</v>
       </c>
       <c r="E15" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F15" t="s">
         <v>19</v>
@@ -1185,18 +1173,18 @@
         <v>1.0397207708399181</v>
       </c>
       <c r="L15" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="M15">
         <v>0</v>
       </c>
       <c r="N15" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B16">
         <v>7.0301000000000005E-7</v>
@@ -1205,7 +1193,7 @@
         <v>7</v>
       </c>
       <c r="E16" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F16" t="s">
         <v>19</v>
@@ -1234,18 +1222,18 @@
         <v>1.0397207708399181</v>
       </c>
       <c r="L16" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="M16">
         <v>0</v>
       </c>
       <c r="N16" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B17">
         <v>5.3800599999999993E-9</v>
@@ -1254,7 +1242,7 @@
         <v>7</v>
       </c>
       <c r="E17" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F17" t="s">
         <v>19</v>
@@ -1283,18 +1271,18 @@
         <v>0.80471895621705025</v>
       </c>
       <c r="L17" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="M17">
         <v>0</v>
       </c>
       <c r="N17" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B18">
         <v>3.0734899999999997E-12</v>
@@ -1303,7 +1291,7 @@
         <v>7</v>
       </c>
       <c r="E18" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F18" t="s">
         <v>19</v>
@@ -1332,18 +1320,18 @@
         <v>0.80471895621705025</v>
       </c>
       <c r="L18" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="M18">
         <v>0</v>
       </c>
       <c r="N18" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B19">
         <v>5.3800599999999993E-6</v>
@@ -1352,7 +1340,7 @@
         <v>7</v>
       </c>
       <c r="E19" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F19" t="s">
         <v>19</v>
@@ -1371,18 +1359,18 @@
         <v>0.80471895621705025</v>
       </c>
       <c r="L19" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="M19">
         <v>0</v>
       </c>
       <c r="N19" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B20" s="6">
         <f>2.65*B42</f>
@@ -1392,7 +1380,7 @@
         <v>7</v>
       </c>
       <c r="E20" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F20" t="s">
         <v>19</v>
@@ -1411,18 +1399,18 @@
         <v>2.439508208471609E-2</v>
       </c>
       <c r="L20" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="M20">
         <v>0</v>
       </c>
       <c r="N20" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B21">
         <v>1.2782000000000001E-5</v>
@@ -1431,7 +1419,7 @@
         <v>7</v>
       </c>
       <c r="E21" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F21" t="s">
         <v>19</v>
@@ -1450,18 +1438,18 @@
         <v>0.20273255405408211</v>
       </c>
       <c r="L21" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="M21">
         <v>0</v>
       </c>
       <c r="N21" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B22">
         <v>5.8099999999999994E-6</v>
@@ -1470,7 +1458,7 @@
         <v>7</v>
       </c>
       <c r="E22" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F22" t="s">
         <v>19</v>
@@ -1489,18 +1477,18 @@
         <v>0.54930614433405478</v>
       </c>
       <c r="L22" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="M22">
         <v>0</v>
       </c>
       <c r="N22" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B23">
         <v>1.6849E-16</v>
@@ -1509,7 +1497,7 @@
         <v>7</v>
       </c>
       <c r="E23" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F23" t="s">
         <v>19</v>
@@ -1528,18 +1516,18 @@
         <v>1.0397207708399181</v>
       </c>
       <c r="L23" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="M23">
         <v>0</v>
       </c>
       <c r="N23" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B24">
         <v>7.9596999999999994E-6</v>
@@ -1548,7 +1536,7 @@
         <v>7</v>
       </c>
       <c r="E24" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F24" t="s">
         <v>19</v>
@@ -1567,18 +1555,18 @@
         <v>0.80471895621705025</v>
       </c>
       <c r="L24" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="M24">
         <v>0</v>
       </c>
       <c r="N24" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B25">
         <v>1.9231099999999998E-7</v>
@@ -1587,7 +1575,7 @@
         <v>7</v>
       </c>
       <c r="E25" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F25" t="s">
         <v>19</v>
@@ -1606,18 +1594,18 @@
         <v>0.80471895621705025</v>
       </c>
       <c r="L25" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="M25">
         <v>0</v>
       </c>
       <c r="N25" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B26">
         <v>3.0502500000000001</v>
@@ -1626,7 +1614,7 @@
         <v>70</v>
       </c>
       <c r="E26" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F26" t="s">
         <v>19</v>
@@ -1645,18 +1633,18 @@
         <v>2.439508208471609E-2</v>
       </c>
       <c r="L26" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="M26">
         <v>0</v>
       </c>
       <c r="N26" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B27">
         <v>4.6073299999999995E-6</v>
@@ -1665,7 +1653,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F27" t="s">
         <v>19</v>
@@ -1684,18 +1672,18 @@
         <v>0.80471895621705025</v>
       </c>
       <c r="L27" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="M27">
         <v>0</v>
       </c>
       <c r="N27" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B28">
         <v>1.7429999999999998E-10</v>
@@ -1704,7 +1692,7 @@
         <v>7</v>
       </c>
       <c r="E28" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F28" t="s">
         <v>19</v>
@@ -1723,13 +1711,13 @@
         <v>0.80471895621705025</v>
       </c>
       <c r="L28" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="M28">
         <v>0</v>
       </c>
       <c r="N28" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
@@ -1743,7 +1731,7 @@
         <v>7</v>
       </c>
       <c r="E29" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F29" t="s">
         <v>19</v>
@@ -1762,18 +1750,18 @@
         <v>0.80471895621705025</v>
       </c>
       <c r="L29" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="M29">
         <v>0</v>
       </c>
       <c r="N29" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B30">
         <v>1.5803199999999998E-4</v>
@@ -1782,7 +1770,7 @@
         <v>7</v>
       </c>
       <c r="E30" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F30" t="s">
         <v>19</v>
@@ -1801,18 +1789,18 @@
         <v>0.20273255405408211</v>
       </c>
       <c r="L30" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="M30">
         <v>0</v>
       </c>
       <c r="N30" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B31">
         <v>4.6479999999999997E-8</v>
@@ -1821,7 +1809,7 @@
         <v>7</v>
       </c>
       <c r="E31" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F31" t="s">
         <v>19</v>
@@ -1840,18 +1828,18 @@
         <v>1.0397207708399181</v>
       </c>
       <c r="L31" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="M31">
         <v>0</v>
       </c>
       <c r="N31" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B32">
         <v>2.9049999999999997E-6</v>
@@ -1860,7 +1848,7 @@
         <v>7</v>
       </c>
       <c r="E32" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F32" t="s">
         <v>19</v>
@@ -1879,18 +1867,18 @@
         <v>0.54930614433405478</v>
       </c>
       <c r="L32" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="M32">
         <v>0</v>
       </c>
       <c r="N32" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B33">
         <v>6.6814999999999995E-6</v>
@@ -1899,7 +1887,7 @@
         <v>7</v>
       </c>
       <c r="E33" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F33" t="s">
         <v>19</v>
@@ -1918,18 +1906,18 @@
         <v>0.80471895621705025</v>
       </c>
       <c r="L33" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="M33">
         <v>0</v>
       </c>
       <c r="N33" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B34">
         <v>4.0960499999999995E-6</v>
@@ -1938,7 +1926,7 @@
         <v>7</v>
       </c>
       <c r="E34" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F34" t="s">
         <v>19</v>
@@ -1957,18 +1945,18 @@
         <v>0.80471895621705025</v>
       </c>
       <c r="L34" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="M34">
         <v>0</v>
       </c>
       <c r="N34" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B35">
         <v>9.2959999999999993E-8</v>
@@ -1977,7 +1965,7 @@
         <v>7</v>
       </c>
       <c r="E35" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F35" t="s">
         <v>19</v>
@@ -1996,13 +1984,13 @@
         <v>1.0397207708399181</v>
       </c>
       <c r="L35" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="M35">
         <v>0</v>
       </c>
       <c r="N35" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
@@ -2016,7 +2004,7 @@
         <v>7</v>
       </c>
       <c r="E36" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F36" t="s">
         <v>19</v>
@@ -2035,18 +2023,18 @@
         <v>4.7655089902162509E-2</v>
       </c>
       <c r="L36" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="M36">
         <v>0</v>
       </c>
       <c r="N36" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B37">
         <v>8.714999999999999E-9</v>
@@ -2055,7 +2043,7 @@
         <v>7</v>
       </c>
       <c r="E37" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F37" t="s">
         <v>19</v>
@@ -2074,18 +2062,18 @@
         <v>0.80471895621705025</v>
       </c>
       <c r="L37" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="M37">
         <v>0</v>
       </c>
       <c r="N37" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B38">
         <v>1.27239E-11</v>
@@ -2097,7 +2085,7 @@
         <v>6</v>
       </c>
       <c r="E38" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F38" t="s">
         <v>35</v>
@@ -2109,7 +2097,7 @@
         <v>-26.847119572100141</v>
       </c>
       <c r="I38">
-        <f t="shared" ref="I15:I43" si="1">LN(SQRT(EXP(
+        <f t="shared" ref="I38:I42" si="1">LN(SQRT(EXP(
 SQRT(
 +POWER(LN(1.05),2)
 +POWER(LN(1.2),2)
@@ -2126,18 +2114,18 @@
         <v>0.3465735902799727</v>
       </c>
       <c r="L38" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="M38">
         <v>0</v>
       </c>
       <c r="N38" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B39">
         <v>1.4525000000000001E-5</v>
@@ -2149,7 +2137,7 @@
         <v>7</v>
       </c>
       <c r="E39" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F39" t="s">
         <v>35</v>
@@ -2168,18 +2156,18 @@
         <v>0.1075556898084728</v>
       </c>
       <c r="L39" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="M39">
         <v>0</v>
       </c>
       <c r="N39" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B40">
         <v>1.1619999999999999E-5</v>
@@ -2191,7 +2179,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F40" t="s">
         <v>35</v>
@@ -2210,30 +2198,30 @@
         <v>0.1075556898084728</v>
       </c>
       <c r="L40" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="M40">
         <v>0</v>
       </c>
       <c r="N40" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B41">
         <v>2.9049999999999998</v>
       </c>
       <c r="C41" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D41" t="s">
         <v>7</v>
       </c>
       <c r="E41" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F41" t="s">
         <v>35</v>
@@ -2252,18 +2240,18 @@
         <v>0.45814536593707761</v>
       </c>
       <c r="L41" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="M41">
         <v>0</v>
       </c>
       <c r="N41" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B42">
         <f>(3.6/47.5)/0.62</f>
@@ -2276,7 +2264,7 @@
         <v>7</v>
       </c>
       <c r="E42" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F42" t="s">
         <v>35</v>
@@ -2295,18 +2283,18 @@
         <v>0</v>
       </c>
       <c r="L42" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="M42">
         <v>0</v>
       </c>
       <c r="N42" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B43">
         <v>-5.8099999999999994E-6</v>
@@ -2318,7 +2306,7 @@
         <v>7</v>
       </c>
       <c r="E43" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="F43" t="s">
         <v>35</v>
@@ -2347,18 +2335,18 @@
         <v>1.0397207708399181</v>
       </c>
       <c r="L43" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="M43">
         <v>0</v>
       </c>
       <c r="N43" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="M44" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="45" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -2366,7 +2354,7 @@
         <v>0</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
@@ -2390,7 +2378,7 @@
         <v>5</v>
       </c>
       <c r="B48" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
@@ -2398,7 +2386,7 @@
         <v>13</v>
       </c>
       <c r="B49" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
@@ -2422,7 +2410,7 @@
         <v>1</v>
       </c>
       <c r="B52" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -2458,7 +2446,7 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B55">
         <v>1</v>
@@ -2476,12 +2464,12 @@
         <v>30</v>
       </c>
       <c r="H55" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B56">
         <v>1.02</v>
@@ -2499,7 +2487,7 @@
         <v>35</v>
       </c>
       <c r="H56" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -2528,7 +2516,7 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B58">
         <f>0.061874*0.669</f>
@@ -2547,12 +2535,12 @@
         <v>35</v>
       </c>
       <c r="H58" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B59">
         <f>0.000000034944*0.669</f>
@@ -2565,18 +2553,18 @@
         <v>69</v>
       </c>
       <c r="F59" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G59" t="s">
         <v>35</v>
       </c>
       <c r="H59" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B60" s="2">
         <v>8.4800000000000005E-8</v>
@@ -2594,12 +2582,12 @@
         <v>35</v>
       </c>
       <c r="H60" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B61">
         <f>(0.00000521*0.669)+0.000010376</f>
@@ -2662,7 +2650,7 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B64">
         <f>0.0000018*0.669</f>
@@ -2686,7 +2674,7 @@
         <v>0</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.2">
@@ -2694,7 +2682,7 @@
         <v>1</v>
       </c>
       <c r="B67" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.2">
@@ -2718,7 +2706,7 @@
         <v>5</v>
       </c>
       <c r="B70" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
@@ -2802,10 +2790,10 @@
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B76" s="5">
-        <v>1.3713596052052344</v>
+        <v>1.6816</v>
       </c>
       <c r="C76" t="s">
         <v>17</v>
@@ -2825,11 +2813,10 @@
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>102</v>
+        <v>22</v>
       </c>
       <c r="B77" s="2">
-        <f>2.65+B76</f>
-        <v>4.0213596052052338</v>
+        <v>5.2130044843049324E-6</v>
       </c>
       <c r="C77" t="s">
         <v>17</v>
@@ -2838,24 +2825,21 @@
         <v>7</v>
       </c>
       <c r="F77" t="s">
-        <v>103</v>
+        <v>18</v>
       </c>
       <c r="G77" t="s">
         <v>19</v>
       </c>
-      <c r="H77" t="s">
-        <v>81</v>
-      </c>
       <c r="I77" t="s">
-        <v>82</v>
+        <v>23</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B78" s="2">
-        <v>5.2130044843049324E-6</v>
+        <v>4.2869955156950664E-4</v>
       </c>
       <c r="C78" t="s">
         <v>17</v>
@@ -2869,16 +2853,19 @@
       <c r="G78" t="s">
         <v>19</v>
       </c>
+      <c r="H78" t="s">
+        <v>25</v>
+      </c>
       <c r="I78" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B79" s="2">
-        <v>4.2869955156950664E-4</v>
+        <v>8.9686098654708509E-6</v>
       </c>
       <c r="C79" t="s">
         <v>17</v>
@@ -2892,19 +2879,16 @@
       <c r="G79" t="s">
         <v>19</v>
       </c>
-      <c r="H79" t="s">
-        <v>25</v>
-      </c>
       <c r="I79" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B80" s="2">
-        <v>8.9686098654708509E-6</v>
+        <v>8.2448430493273531E-4</v>
       </c>
       <c r="C80" t="s">
         <v>17</v>
@@ -2919,64 +2903,70 @@
         <v>19</v>
       </c>
       <c r="I80" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>27</v>
-      </c>
-      <c r="B81" s="2">
-        <v>8.2448430493273531E-4</v>
+        <v>100</v>
+      </c>
+      <c r="B81">
+        <v>1</v>
       </c>
       <c r="C81" t="s">
-        <v>17</v>
+        <v>29</v>
+      </c>
+      <c r="D81" t="s">
+        <v>58</v>
       </c>
       <c r="E81" t="s">
         <v>7</v>
       </c>
-      <c r="F81" t="s">
-        <v>18</v>
-      </c>
       <c r="G81" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="I81" t="s">
-        <v>28</v>
+        <v>5</v>
+      </c>
+      <c r="J81" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>104</v>
-      </c>
-      <c r="B82">
-        <v>1</v>
+        <v>32</v>
+      </c>
+      <c r="B82" s="2">
+        <v>2.8160765678334782E-2</v>
       </c>
       <c r="C82" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D82" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="E82" t="s">
         <v>7</v>
       </c>
       <c r="G82" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="I82" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="J82" t="s">
-        <v>31</v>
+        <v>37</v>
+      </c>
+      <c r="K82" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B83" s="2">
-        <v>2.8160765678334782E-2</v>
+        <v>1.1043437520915599E-3</v>
       </c>
       <c r="C83" t="s">
         <v>33</v>
@@ -2991,10 +2981,10 @@
         <v>35</v>
       </c>
       <c r="I83" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="J83" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="K83" t="s">
         <v>38</v>
@@ -3002,10 +2992,10 @@
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B84" s="2">
-        <v>1.1043437520915599E-3</v>
+        <v>5.9790732436472346E-10</v>
       </c>
       <c r="C84" t="s">
         <v>33</v>
@@ -3014,27 +3004,27 @@
         <v>34</v>
       </c>
       <c r="E84" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G84" t="s">
         <v>35</v>
       </c>
       <c r="I84" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="J84" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="K84" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B85" s="2">
-        <v>5.9790732436472346E-10</v>
+        <v>6.6260625125493598E-5</v>
       </c>
       <c r="C85" t="s">
         <v>33</v>
@@ -3043,33 +3033,33 @@
         <v>34</v>
       </c>
       <c r="E85" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G85" t="s">
         <v>35</v>
       </c>
       <c r="I85" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="J85" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="K85" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B86" s="2">
-        <v>6.6260625125493598E-5</v>
+        <v>6.6260625125493591E-2</v>
       </c>
       <c r="C86" t="s">
         <v>33</v>
       </c>
       <c r="D86" t="s">
-        <v>34</v>
+        <v>69</v>
       </c>
       <c r="E86" t="s">
         <v>7</v>
@@ -3077,291 +3067,288 @@
       <c r="G86" t="s">
         <v>35</v>
       </c>
-      <c r="I86" t="s">
-        <v>47</v>
-      </c>
       <c r="J86" t="s">
-        <v>48</v>
-      </c>
-      <c r="K86" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B87" s="2">
-        <v>6.6260625125493591E-2</v>
+        <v>0.17937219730941703</v>
       </c>
       <c r="C87" t="s">
         <v>33</v>
       </c>
       <c r="D87" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="E87" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="G87" t="s">
         <v>35</v>
       </c>
+      <c r="H87" t="s">
+        <v>53</v>
+      </c>
+      <c r="I87" t="s">
+        <v>54</v>
+      </c>
       <c r="J87" t="s">
-        <v>50</v>
+        <v>55</v>
+      </c>
+      <c r="K87" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="B88" s="2">
-        <v>0.17937219730941703</v>
+        <v>1.1457566427949933E-2</v>
       </c>
       <c r="C88" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D88" t="s">
         <v>58</v>
       </c>
       <c r="E88" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="G88" t="s">
         <v>35</v>
       </c>
-      <c r="H88" t="s">
-        <v>53</v>
-      </c>
       <c r="I88" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="J88" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="K88" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B89" s="2">
-        <v>1.1457566427949933E-2</v>
+        <v>2.20868750418312</v>
       </c>
       <c r="C89" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D89" t="s">
-        <v>58</v>
+        <v>3</v>
       </c>
       <c r="E89" t="s">
-        <v>7</v>
+        <v>62</v>
       </c>
       <c r="G89" t="s">
         <v>35</v>
       </c>
-      <c r="I89" t="s">
-        <v>59</v>
-      </c>
       <c r="J89" t="s">
-        <v>60</v>
-      </c>
-      <c r="K89" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>61</v>
-      </c>
-      <c r="B90" s="2">
-        <v>2.20868750418312</v>
+        <v>96</v>
+      </c>
+      <c r="B90">
+        <v>55.5</v>
       </c>
       <c r="C90" t="s">
-        <v>33</v>
-      </c>
-      <c r="D90" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="E90" t="s">
-        <v>62</v>
+        <v>70</v>
+      </c>
+      <c r="F90" t="s">
+        <v>97</v>
       </c>
       <c r="G90" t="s">
-        <v>35</v>
-      </c>
-      <c r="J90" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
-        <v>98</v>
-      </c>
-      <c r="B91">
-        <v>55.5</v>
-      </c>
-      <c r="C91" t="s">
-        <v>17</v>
-      </c>
-      <c r="E91" t="s">
-        <v>70</v>
-      </c>
-      <c r="F91" t="s">
-        <v>99</v>
-      </c>
-      <c r="G91" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="93" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A93" s="1" t="s">
+    <row r="92" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A92" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B93" s="1" t="s">
+      <c r="B92" s="1" t="s">
         <v>57</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>64</v>
+      </c>
+      <c r="B93" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>64</v>
+        <v>2</v>
       </c>
       <c r="B94" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>2</v>
-      </c>
-      <c r="B95" t="s">
-        <v>58</v>
+        <v>4</v>
+      </c>
+      <c r="B95">
+        <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>4</v>
-      </c>
-      <c r="B96">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="B96" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B97" t="s">
-        <v>60</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="M97" s="2"/>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="B98" t="s">
-        <v>7</v>
-      </c>
-      <c r="M98" s="2"/>
+        <v>29</v>
+      </c>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="B99" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A100" t="s">
-        <v>79</v>
-      </c>
-      <c r="B100" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="101" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A101" s="1" t="s">
+    <row r="100" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A100" s="1" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>9</v>
+      </c>
+      <c r="B101" t="s">
+        <v>10</v>
+      </c>
+      <c r="C101" t="s">
+        <v>11</v>
+      </c>
+      <c r="D101" t="s">
+        <v>2</v>
+      </c>
+      <c r="E101" t="s">
+        <v>6</v>
+      </c>
+      <c r="F101" t="s">
+        <v>13</v>
+      </c>
+      <c r="G101" t="s">
+        <v>67</v>
+      </c>
+      <c r="H101" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>9</v>
-      </c>
-      <c r="B102" t="s">
-        <v>10</v>
+        <v>57</v>
+      </c>
+      <c r="B102">
+        <v>1</v>
       </c>
       <c r="C102" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="D102" t="s">
-        <v>2</v>
+        <v>58</v>
       </c>
       <c r="E102" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F102" t="s">
-        <v>13</v>
-      </c>
-      <c r="G102" t="s">
-        <v>67</v>
+        <v>30</v>
       </c>
       <c r="H102" t="s">
-        <v>5</v>
+        <v>60</v>
       </c>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="B103">
-        <v>1</v>
+        <v>2.3800000000000001E-4</v>
       </c>
       <c r="C103" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D103" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="E103" t="s">
-        <v>7</v>
+        <v>70</v>
       </c>
       <c r="F103" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H103" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B104">
-        <v>2.3800000000000001E-4</v>
+        <v>3.4339655648031599E-10</v>
       </c>
       <c r="C104" t="s">
         <v>33</v>
       </c>
       <c r="D104" t="s">
-        <v>69</v>
+        <v>34</v>
       </c>
       <c r="E104" t="s">
-        <v>70</v>
+        <v>7</v>
       </c>
       <c r="F104" t="s">
         <v>35</v>
       </c>
+      <c r="G104" t="s">
+        <v>73</v>
+      </c>
       <c r="H104" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B105">
-        <v>3.4339655648031599E-10</v>
+        <v>1.8660000000000003E-2</v>
       </c>
       <c r="C105" t="s">
         <v>33</v>
@@ -3375,19 +3362,16 @@
       <c r="F105" t="s">
         <v>35</v>
       </c>
-      <c r="G105" t="s">
-        <v>73</v>
-      </c>
       <c r="H105" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B106">
-        <v>1.8660000000000003E-2</v>
+        <v>8.1000000000000013E-3</v>
       </c>
       <c r="C106" t="s">
         <v>33</v>
@@ -3402,21 +3386,21 @@
         <v>35</v>
       </c>
       <c r="H106" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>77</v>
+        <v>49</v>
       </c>
       <c r="B107">
-        <v>8.1000000000000013E-3</v>
+        <v>0.996</v>
       </c>
       <c r="C107" t="s">
         <v>33</v>
       </c>
       <c r="D107" t="s">
-        <v>34</v>
+        <v>69</v>
       </c>
       <c r="E107" t="s">
         <v>7</v>
@@ -3425,52 +3409,29 @@
         <v>35</v>
       </c>
       <c r="H107" t="s">
-        <v>78</v>
+        <v>50</v>
       </c>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B108">
-        <v>0.996</v>
+        <v>3.44E-2</v>
       </c>
       <c r="C108" t="s">
         <v>33</v>
       </c>
       <c r="D108" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="E108" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="F108" t="s">
         <v>35</v>
       </c>
       <c r="H108" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A109" t="s">
-        <v>51</v>
-      </c>
-      <c r="B109">
-        <v>3.44E-2</v>
-      </c>
-      <c r="C109" t="s">
-        <v>33</v>
-      </c>
-      <c r="D109" t="s">
-        <v>58</v>
-      </c>
-      <c r="E109" t="s">
-        <v>52</v>
-      </c>
-      <c r="F109" t="s">
-        <v>35</v>
-      </c>
-      <c r="H109" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix a few LCIs
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-biogas.xlsx
+++ b/premise/data/additional_inventories/lci-biogas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D6A4F86-13C1-3845-8416-3508BA4018C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9236AF5-8C66-924B-AAEA-6E6BB4C6DC03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34720" yWindow="160" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1160" yWindow="1080" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Biogas" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="156">
   <si>
     <t>Activity</t>
   </si>
@@ -335,9 +335,6 @@
   </si>
   <si>
     <t>Density: 0.669 kg/Nm3, LHV: 47.5 MJ/kg</t>
-  </si>
-  <si>
-    <t>electricity production, at natural gas-fired combined cycle power plant</t>
   </si>
   <si>
     <t/>
@@ -889,8 +886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="A127" sqref="A127"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -917,10 +914,10 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="M3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
@@ -931,7 +928,7 @@
         <v>58</v>
       </c>
       <c r="M4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -942,7 +939,7 @@
         <v>1</v>
       </c>
       <c r="M5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -950,7 +947,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -958,7 +955,7 @@
         <v>79</v>
       </c>
       <c r="B7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
@@ -969,7 +966,7 @@
         <v>85</v>
       </c>
       <c r="M8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
@@ -980,7 +977,7 @@
         <v>81</v>
       </c>
       <c r="M9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
@@ -991,7 +988,7 @@
         <v>52</v>
       </c>
       <c r="M10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -999,7 +996,7 @@
         <v>8</v>
       </c>
       <c r="M11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
@@ -1022,33 +1019,34 @@
         <v>13</v>
       </c>
       <c r="G12" t="s">
+        <v>102</v>
+      </c>
+      <c r="H12" t="s">
         <v>103</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
+        <v>155</v>
+      </c>
+      <c r="J12" t="s">
         <v>104</v>
-      </c>
-      <c r="I12" t="s">
-        <v>156</v>
-      </c>
-      <c r="J12" t="s">
-        <v>105</v>
       </c>
       <c r="K12" t="s">
         <v>1</v>
       </c>
       <c r="L12" t="s">
+        <v>105</v>
+      </c>
+      <c r="M12" t="s">
         <v>106</v>
-      </c>
-      <c r="M12" t="s">
-        <v>107</v>
       </c>
       <c r="N12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>101</v>
+      <c r="A13" t="str">
+        <f>B3</f>
+        <v>electricity production, at biomethane-fired combined cycle power plant</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -1060,7 +1058,7 @@
         <v>52</v>
       </c>
       <c r="E13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F13" t="s">
         <v>30</v>
@@ -1069,18 +1067,19 @@
         <v>100</v>
       </c>
       <c r="K13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L13" t="s">
-        <v>109</v>
-      </c>
-      <c r="N13" t="s">
-        <v>102</v>
+        <v>108</v>
+      </c>
+      <c r="N13" t="str">
+        <f>B8</f>
+        <v>electricity, high voltage</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B14">
         <v>4.6073299999999991E-12</v>
@@ -1089,7 +1088,7 @@
         <v>7</v>
       </c>
       <c r="E14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F14" t="s">
         <v>19</v>
@@ -1118,18 +1117,18 @@
         <v>0.80471895621705025</v>
       </c>
       <c r="L14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="M14">
         <v>0</v>
       </c>
       <c r="N14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B15">
         <v>4.6479999999999997E-9</v>
@@ -1138,7 +1137,7 @@
         <v>7</v>
       </c>
       <c r="E15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F15" t="s">
         <v>19</v>
@@ -1167,18 +1166,18 @@
         <v>1.0397207708399181</v>
       </c>
       <c r="L15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M15">
         <v>0</v>
       </c>
       <c r="N15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B16">
         <v>7.0301000000000005E-7</v>
@@ -1187,7 +1186,7 @@
         <v>7</v>
       </c>
       <c r="E16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F16" t="s">
         <v>19</v>
@@ -1216,18 +1215,18 @@
         <v>1.0397207708399181</v>
       </c>
       <c r="L16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M16">
         <v>0</v>
       </c>
       <c r="N16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B17">
         <v>5.3800599999999993E-9</v>
@@ -1236,7 +1235,7 @@
         <v>7</v>
       </c>
       <c r="E17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F17" t="s">
         <v>19</v>
@@ -1265,18 +1264,18 @@
         <v>0.80471895621705025</v>
       </c>
       <c r="L17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="M17">
         <v>0</v>
       </c>
       <c r="N17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B18">
         <v>3.0734899999999997E-12</v>
@@ -1285,7 +1284,7 @@
         <v>7</v>
       </c>
       <c r="E18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F18" t="s">
         <v>19</v>
@@ -1314,18 +1313,18 @@
         <v>0.80471895621705025</v>
       </c>
       <c r="L18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="M18">
         <v>0</v>
       </c>
       <c r="N18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B19">
         <v>5.3800599999999993E-6</v>
@@ -1334,7 +1333,7 @@
         <v>7</v>
       </c>
       <c r="E19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F19" t="s">
         <v>19</v>
@@ -1353,13 +1352,13 @@
         <v>0.80471895621705025</v>
       </c>
       <c r="L19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="M19">
         <v>0</v>
       </c>
       <c r="N19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
@@ -1374,7 +1373,7 @@
         <v>7</v>
       </c>
       <c r="E20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F20" t="s">
         <v>19</v>
@@ -1393,13 +1392,13 @@
         <v>2.439508208471609E-2</v>
       </c>
       <c r="L20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="M20">
         <v>0</v>
       </c>
       <c r="N20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
@@ -1413,7 +1412,7 @@
         <v>7</v>
       </c>
       <c r="E21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F21" t="s">
         <v>19</v>
@@ -1432,18 +1431,18 @@
         <v>0.20273255405408211</v>
       </c>
       <c r="L21" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="M21">
         <v>0</v>
       </c>
       <c r="N21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B22">
         <v>5.8099999999999994E-6</v>
@@ -1452,7 +1451,7 @@
         <v>7</v>
       </c>
       <c r="E22" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F22" t="s">
         <v>19</v>
@@ -1471,18 +1470,18 @@
         <v>0.54930614433405478</v>
       </c>
       <c r="L22" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M22">
         <v>0</v>
       </c>
       <c r="N22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B23">
         <v>1.6849E-16</v>
@@ -1491,7 +1490,7 @@
         <v>7</v>
       </c>
       <c r="E23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F23" t="s">
         <v>19</v>
@@ -1510,18 +1509,18 @@
         <v>1.0397207708399181</v>
       </c>
       <c r="L23" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M23">
         <v>0</v>
       </c>
       <c r="N23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B24">
         <v>7.9596999999999994E-6</v>
@@ -1530,7 +1529,7 @@
         <v>7</v>
       </c>
       <c r="E24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F24" t="s">
         <v>19</v>
@@ -1549,18 +1548,18 @@
         <v>0.80471895621705025</v>
       </c>
       <c r="L24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="M24">
         <v>0</v>
       </c>
       <c r="N24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B25">
         <v>1.9231099999999998E-7</v>
@@ -1569,7 +1568,7 @@
         <v>7</v>
       </c>
       <c r="E25" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F25" t="s">
         <v>19</v>
@@ -1588,18 +1587,18 @@
         <v>0.80471895621705025</v>
       </c>
       <c r="L25" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="M25">
         <v>0</v>
       </c>
       <c r="N25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B26">
         <v>3.0502500000000001</v>
@@ -1608,7 +1607,7 @@
         <v>70</v>
       </c>
       <c r="E26" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F26" t="s">
         <v>19</v>
@@ -1627,18 +1626,18 @@
         <v>2.439508208471609E-2</v>
       </c>
       <c r="L26" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="M26">
         <v>0</v>
       </c>
       <c r="N26" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B27">
         <v>4.6073299999999995E-6</v>
@@ -1647,7 +1646,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F27" t="s">
         <v>19</v>
@@ -1666,18 +1665,18 @@
         <v>0.80471895621705025</v>
       </c>
       <c r="L27" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="M27">
         <v>0</v>
       </c>
       <c r="N27" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B28">
         <v>1.7429999999999998E-10</v>
@@ -1686,7 +1685,7 @@
         <v>7</v>
       </c>
       <c r="E28" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F28" t="s">
         <v>19</v>
@@ -1705,13 +1704,13 @@
         <v>0.80471895621705025</v>
       </c>
       <c r="L28" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="M28">
         <v>0</v>
       </c>
       <c r="N28" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
@@ -1725,7 +1724,7 @@
         <v>7</v>
       </c>
       <c r="E29" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F29" t="s">
         <v>19</v>
@@ -1744,13 +1743,13 @@
         <v>0.80471895621705025</v>
       </c>
       <c r="L29" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="M29">
         <v>0</v>
       </c>
       <c r="N29" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
@@ -1764,7 +1763,7 @@
         <v>7</v>
       </c>
       <c r="E30" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F30" t="s">
         <v>19</v>
@@ -1783,18 +1782,18 @@
         <v>0.20273255405408211</v>
       </c>
       <c r="L30" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="M30">
         <v>0</v>
       </c>
       <c r="N30" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B31">
         <v>4.6479999999999997E-8</v>
@@ -1803,7 +1802,7 @@
         <v>7</v>
       </c>
       <c r="E31" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F31" t="s">
         <v>19</v>
@@ -1822,13 +1821,13 @@
         <v>1.0397207708399181</v>
       </c>
       <c r="L31" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M31">
         <v>0</v>
       </c>
       <c r="N31" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
@@ -1842,7 +1841,7 @@
         <v>7</v>
       </c>
       <c r="E32" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F32" t="s">
         <v>19</v>
@@ -1861,18 +1860,18 @@
         <v>0.54930614433405478</v>
       </c>
       <c r="L32" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M32">
         <v>0</v>
       </c>
       <c r="N32" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B33">
         <v>6.6814999999999995E-6</v>
@@ -1881,7 +1880,7 @@
         <v>7</v>
       </c>
       <c r="E33" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F33" t="s">
         <v>19</v>
@@ -1900,18 +1899,18 @@
         <v>0.80471895621705025</v>
       </c>
       <c r="L33" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="M33">
         <v>0</v>
       </c>
       <c r="N33" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B34">
         <v>4.0960499999999995E-6</v>
@@ -1920,7 +1919,7 @@
         <v>7</v>
       </c>
       <c r="E34" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F34" t="s">
         <v>19</v>
@@ -1939,18 +1938,18 @@
         <v>0.80471895621705025</v>
       </c>
       <c r="L34" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="M34">
         <v>0</v>
       </c>
       <c r="N34" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B35">
         <v>9.2959999999999993E-8</v>
@@ -1959,7 +1958,7 @@
         <v>7</v>
       </c>
       <c r="E35" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F35" t="s">
         <v>19</v>
@@ -1978,13 +1977,13 @@
         <v>1.0397207708399181</v>
       </c>
       <c r="L35" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M35">
         <v>0</v>
       </c>
       <c r="N35" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
@@ -1998,7 +1997,7 @@
         <v>7</v>
       </c>
       <c r="E36" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F36" t="s">
         <v>19</v>
@@ -2017,18 +2016,18 @@
         <v>4.7655089902162509E-2</v>
       </c>
       <c r="L36" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="M36">
         <v>0</v>
       </c>
       <c r="N36" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B37">
         <v>8.714999999999999E-9</v>
@@ -2037,7 +2036,7 @@
         <v>7</v>
       </c>
       <c r="E37" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F37" t="s">
         <v>19</v>
@@ -2056,18 +2055,18 @@
         <v>0.80471895621705025</v>
       </c>
       <c r="L37" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="M37">
         <v>0</v>
       </c>
       <c r="N37" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B38">
         <v>1.27239E-11</v>
@@ -2079,7 +2078,7 @@
         <v>6</v>
       </c>
       <c r="E38" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F38" t="s">
         <v>35</v>
@@ -2108,18 +2107,18 @@
         <v>0.3465735902799727</v>
       </c>
       <c r="L38" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M38">
         <v>0</v>
       </c>
       <c r="N38" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B39">
         <v>1.4525000000000001E-5</v>
@@ -2131,7 +2130,7 @@
         <v>7</v>
       </c>
       <c r="E39" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F39" t="s">
         <v>35</v>
@@ -2150,18 +2149,18 @@
         <v>0.1075556898084728</v>
       </c>
       <c r="L39" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M39">
         <v>0</v>
       </c>
       <c r="N39" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B40">
         <v>1.1619999999999999E-5</v>
@@ -2173,7 +2172,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F40" t="s">
         <v>35</v>
@@ -2192,30 +2191,30 @@
         <v>0.1075556898084728</v>
       </c>
       <c r="L40" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M40">
         <v>0</v>
       </c>
       <c r="N40" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B41">
         <v>2.9049999999999998</v>
       </c>
       <c r="C41" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D41" t="s">
         <v>7</v>
       </c>
       <c r="E41" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F41" t="s">
         <v>35</v>
@@ -2234,13 +2233,13 @@
         <v>0.45814536593707761</v>
       </c>
       <c r="L41" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="M41">
         <v>0</v>
       </c>
       <c r="N41" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
@@ -2258,7 +2257,7 @@
         <v>7</v>
       </c>
       <c r="E42" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F42" t="s">
         <v>35</v>
@@ -2277,7 +2276,7 @@
         <v>0</v>
       </c>
       <c r="L42" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M42">
         <v>0</v>
@@ -2288,7 +2287,7 @@
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B43">
         <v>-5.8099999999999994E-6</v>
@@ -2300,7 +2299,7 @@
         <v>7</v>
       </c>
       <c r="E43" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F43" t="s">
         <v>35</v>
@@ -2329,18 +2328,18 @@
         <v>1.0397207708399181</v>
       </c>
       <c r="L43" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M43">
         <v>0</v>
       </c>
       <c r="N43" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="M44" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="45" spans="1:14" ht="16" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Fix uncertainty data in LCIs
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-biogas.xlsx
+++ b/premise/data/additional_inventories/lci-biogas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/Github/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9236AF5-8C66-924B-AAEA-6E6BB4C6DC03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C173779-419C-784C-8CFA-56D5F17DB146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="1080" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -588,9 +588,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -628,7 +628,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -734,7 +734,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -876,7 +876,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -886,8 +886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1119,9 +1119,6 @@
       <c r="L14" t="s">
         <v>111</v>
       </c>
-      <c r="M14">
-        <v>0</v>
-      </c>
       <c r="N14" t="s">
         <v>101</v>
       </c>
@@ -1168,9 +1165,6 @@
       <c r="L15" t="s">
         <v>113</v>
       </c>
-      <c r="M15">
-        <v>0</v>
-      </c>
       <c r="N15" t="s">
         <v>101</v>
       </c>
@@ -1217,9 +1211,6 @@
       <c r="L16" t="s">
         <v>113</v>
       </c>
-      <c r="M16">
-        <v>0</v>
-      </c>
       <c r="N16" t="s">
         <v>101</v>
       </c>
@@ -1266,9 +1257,6 @@
       <c r="L17" t="s">
         <v>111</v>
       </c>
-      <c r="M17">
-        <v>0</v>
-      </c>
       <c r="N17" t="s">
         <v>101</v>
       </c>
@@ -1315,9 +1303,6 @@
       <c r="L18" t="s">
         <v>111</v>
       </c>
-      <c r="M18">
-        <v>0</v>
-      </c>
       <c r="N18" t="s">
         <v>101</v>
       </c>
@@ -1354,9 +1339,6 @@
       <c r="L19" t="s">
         <v>111</v>
       </c>
-      <c r="M19">
-        <v>0</v>
-      </c>
       <c r="N19" t="s">
         <v>101</v>
       </c>
@@ -1394,9 +1376,6 @@
       <c r="L20" t="s">
         <v>118</v>
       </c>
-      <c r="M20">
-        <v>0</v>
-      </c>
       <c r="N20" t="s">
         <v>101</v>
       </c>
@@ -1433,9 +1412,6 @@
       <c r="L21" t="s">
         <v>119</v>
       </c>
-      <c r="M21">
-        <v>0</v>
-      </c>
       <c r="N21" t="s">
         <v>101</v>
       </c>
@@ -1472,9 +1448,6 @@
       <c r="L22" t="s">
         <v>121</v>
       </c>
-      <c r="M22">
-        <v>0</v>
-      </c>
       <c r="N22" t="s">
         <v>101</v>
       </c>
@@ -1511,9 +1484,6 @@
       <c r="L23" t="s">
         <v>113</v>
       </c>
-      <c r="M23">
-        <v>0</v>
-      </c>
       <c r="N23" t="s">
         <v>101</v>
       </c>
@@ -1550,9 +1520,6 @@
       <c r="L24" t="s">
         <v>111</v>
       </c>
-      <c r="M24">
-        <v>0</v>
-      </c>
       <c r="N24" t="s">
         <v>101</v>
       </c>
@@ -1589,9 +1556,6 @@
       <c r="L25" t="s">
         <v>111</v>
       </c>
-      <c r="M25">
-        <v>0</v>
-      </c>
       <c r="N25" t="s">
         <v>101</v>
       </c>
@@ -1628,9 +1592,6 @@
       <c r="L26" t="s">
         <v>126</v>
       </c>
-      <c r="M26">
-        <v>0</v>
-      </c>
       <c r="N26" t="s">
         <v>101</v>
       </c>
@@ -1667,9 +1628,6 @@
       <c r="L27" t="s">
         <v>111</v>
       </c>
-      <c r="M27">
-        <v>0</v>
-      </c>
       <c r="N27" t="s">
         <v>101</v>
       </c>
@@ -1706,9 +1664,6 @@
       <c r="L28" t="s">
         <v>129</v>
       </c>
-      <c r="M28">
-        <v>0</v>
-      </c>
       <c r="N28" t="s">
         <v>101</v>
       </c>
@@ -1745,9 +1700,6 @@
       <c r="L29" t="s">
         <v>130</v>
       </c>
-      <c r="M29">
-        <v>0</v>
-      </c>
       <c r="N29" t="s">
         <v>101</v>
       </c>
@@ -1784,9 +1736,6 @@
       <c r="L30" t="s">
         <v>131</v>
       </c>
-      <c r="M30">
-        <v>0</v>
-      </c>
       <c r="N30" t="s">
         <v>101</v>
       </c>
@@ -1823,9 +1772,6 @@
       <c r="L31" t="s">
         <v>113</v>
       </c>
-      <c r="M31">
-        <v>0</v>
-      </c>
       <c r="N31" t="s">
         <v>101</v>
       </c>
@@ -1862,9 +1808,6 @@
       <c r="L32" t="s">
         <v>121</v>
       </c>
-      <c r="M32">
-        <v>0</v>
-      </c>
       <c r="N32" t="s">
         <v>101</v>
       </c>
@@ -1901,9 +1844,6 @@
       <c r="L33" t="s">
         <v>111</v>
       </c>
-      <c r="M33">
-        <v>0</v>
-      </c>
       <c r="N33" t="s">
         <v>101</v>
       </c>
@@ -1940,9 +1880,6 @@
       <c r="L34" t="s">
         <v>111</v>
       </c>
-      <c r="M34">
-        <v>0</v>
-      </c>
       <c r="N34" t="s">
         <v>101</v>
       </c>
@@ -1979,9 +1916,6 @@
       <c r="L35" t="s">
         <v>113</v>
       </c>
-      <c r="M35">
-        <v>0</v>
-      </c>
       <c r="N35" t="s">
         <v>101</v>
       </c>
@@ -2018,9 +1952,6 @@
       <c r="L36" t="s">
         <v>118</v>
       </c>
-      <c r="M36">
-        <v>0</v>
-      </c>
       <c r="N36" t="s">
         <v>101</v>
       </c>
@@ -2056,9 +1987,6 @@
       </c>
       <c r="L37" t="s">
         <v>111</v>
-      </c>
-      <c r="M37">
-        <v>0</v>
       </c>
       <c r="N37" t="s">
         <v>101</v>
@@ -2109,9 +2037,6 @@
       <c r="L38" t="s">
         <v>139</v>
       </c>
-      <c r="M38">
-        <v>0</v>
-      </c>
       <c r="N38" t="s">
         <v>140</v>
       </c>
@@ -2151,9 +2076,6 @@
       <c r="L39" t="s">
         <v>142</v>
       </c>
-      <c r="M39">
-        <v>0</v>
-      </c>
       <c r="N39" t="s">
         <v>143</v>
       </c>
@@ -2193,9 +2115,6 @@
       <c r="L40" t="s">
         <v>142</v>
       </c>
-      <c r="M40">
-        <v>0</v>
-      </c>
       <c r="N40" t="s">
         <v>145</v>
       </c>
@@ -2235,9 +2154,6 @@
       <c r="L41" t="s">
         <v>130</v>
       </c>
-      <c r="M41">
-        <v>0</v>
-      </c>
       <c r="N41" t="s">
         <v>153</v>
       </c>
@@ -2278,9 +2194,6 @@
       <c r="L42" t="s">
         <v>101</v>
       </c>
-      <c r="M42">
-        <v>0</v>
-      </c>
       <c r="N42" t="s">
         <v>99</v>
       </c>
@@ -2308,7 +2221,8 @@
         <v>2</v>
       </c>
       <c r="H43">
-        <v>-13.81551055796427</v>
+        <f>LN(B43*-1)</f>
+        <v>-12.055929987100454</v>
       </c>
       <c r="I43">
         <f>LN(SQRT(EXP(
@@ -2330,8 +2244,8 @@
       <c r="L43" t="s">
         <v>113</v>
       </c>
-      <c r="M43">
-        <v>0</v>
+      <c r="M43" t="b">
+        <v>1</v>
       </c>
       <c r="N43" t="s">
         <v>148</v>

</xml_diff>